<commit_message>
Update codebook and fix more coding mistakes
</commit_message>
<xml_diff>
--- a/case codings database.xlsx
+++ b/case codings database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Studium\Bachelor's Thesis\ucf-thesis-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF36CEC0-ADEF-4FCE-BDC5-3FC6163562CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5862D81-14E2-4A92-A6D8-33CDD9F8C528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7785" yWindow="-13230" windowWidth="23010" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="-14955" windowWidth="23010" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="244">
   <si>
     <t>ID</t>
   </si>
@@ -390,9 +390,6 @@
     <t>2 = Clear chain of command and decision-making apparatus maintained at all times</t>
   </si>
   <si>
-    <t>2 = Yes, they used alternative strategies before the use of force in question.</t>
-  </si>
-  <si>
     <t>Anik and Others v. Turkey</t>
   </si>
   <si>
@@ -594,9 +591,6 @@
     <t>Gülen v. Turkey</t>
   </si>
   <si>
-    <t>1 = Yes, they considered the use of alternative strategies</t>
-  </si>
-  <si>
     <t>Gülşenoğlu v. Turkey</t>
   </si>
   <si>
@@ -760,6 +754,9 @@
   </si>
   <si>
     <t>Yüksel Erdoğan and Others v. Turkey</t>
+  </si>
+  <si>
+    <t>1 = Yes, they considered or used alternative strategies before the use of force in question</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="AM64" workbookViewId="0">
+      <selection activeCell="AQ44" sqref="AQ44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2156,7 +2153,7 @@
         <v>85</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>60</v>
@@ -2556,7 +2553,7 @@
         <v>120</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR8" s="2" t="s">
         <v>60</v>
@@ -2588,10 +2585,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>81</v>
@@ -2672,7 +2669,7 @@
         <v>101</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE9" s="2" t="s">
         <v>68</v>
@@ -2743,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>53</v>
@@ -2758,7 +2755,7 @@
         <v>54</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>56</v>
@@ -2827,7 +2824,7 @@
         <v>89</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>68</v>
@@ -2898,7 +2895,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>106</v>
@@ -2931,7 +2928,7 @@
         <v>58</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>60</v>
@@ -2997,16 +2994,16 @@
         <v>102</v>
       </c>
       <c r="AI11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL11" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="AJ11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL11" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="AM11" s="2" t="s">
         <v>68</v>
@@ -3053,10 +3050,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>81</v>
@@ -3068,7 +3065,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>56</v>
@@ -3146,10 +3143,10 @@
         <v>112</v>
       </c>
       <c r="AG12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH12" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="AH12" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="AI12" s="2" t="s">
         <v>91</v>
@@ -3194,7 +3191,7 @@
         <v>68</v>
       </c>
       <c r="AW12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX12" s="2" t="s">
         <v>54</v>
@@ -3208,10 +3205,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>81</v>
@@ -3292,7 +3289,7 @@
         <v>101</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE13" s="2" t="s">
         <v>68</v>
@@ -3316,7 +3313,7 @@
         <v>92</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM13" s="2" t="s">
         <v>68</v>
@@ -3363,14 +3360,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="E14" s="2" t="s">
         <v>54</v>
       </c>
@@ -3378,7 +3375,7 @@
         <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>56</v>
@@ -3444,22 +3441,22 @@
         <v>100</v>
       </c>
       <c r="AC14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD14" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AE14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH14" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="AI14" s="2" t="s">
         <v>91</v>
@@ -3486,7 +3483,7 @@
         <v>120</v>
       </c>
       <c r="AQ14" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR14" s="2" t="s">
         <v>60</v>
@@ -3518,10 +3515,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>81</v>
@@ -3533,7 +3530,7 @@
         <v>54</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>56</v>
@@ -3617,7 +3614,7 @@
         <v>72</v>
       </c>
       <c r="AI15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ15" s="2" t="s">
         <v>60</v>
@@ -3673,13 +3670,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>54</v>
@@ -3757,7 +3754,7 @@
         <v>101</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE16" s="2" t="s">
         <v>68</v>
@@ -3766,10 +3763,10 @@
         <v>68</v>
       </c>
       <c r="AG16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AI16" s="2" t="s">
         <v>91</v>
@@ -3781,7 +3778,7 @@
         <v>54</v>
       </c>
       <c r="AL16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM16" s="2" t="s">
         <v>103</v>
@@ -3796,7 +3793,7 @@
         <v>120</v>
       </c>
       <c r="AQ16" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR16" s="2" t="s">
         <v>68</v>
@@ -3805,7 +3802,7 @@
         <v>68</v>
       </c>
       <c r="AT16" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU16" s="2" t="s">
         <v>68</v>
@@ -3828,22 +3825,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>83</v>
@@ -3921,10 +3918,10 @@
         <v>68</v>
       </c>
       <c r="AG17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI17" s="2" t="s">
         <v>91</v>
@@ -3933,7 +3930,7 @@
         <v>54</v>
       </c>
       <c r="AK17" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL17" s="2" t="s">
         <v>74</v>
@@ -3951,7 +3948,7 @@
         <v>120</v>
       </c>
       <c r="AQ17" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR17" s="2" t="s">
         <v>60</v>
@@ -3960,7 +3957,7 @@
         <v>60</v>
       </c>
       <c r="AT17" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU17" s="2" t="s">
         <v>68</v>
@@ -3969,7 +3966,7 @@
         <v>68</v>
       </c>
       <c r="AW17" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX17" s="2" t="s">
         <v>60</v>
@@ -3983,10 +3980,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>81</v>
@@ -4070,7 +4067,7 @@
         <v>68</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AF18" s="2" t="s">
         <v>62</v>
@@ -4082,7 +4079,7 @@
         <v>72</v>
       </c>
       <c r="AI18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ18" s="2" t="s">
         <v>54</v>
@@ -4138,13 +4135,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>54</v>
@@ -4198,10 +4195,10 @@
         <v>54</v>
       </c>
       <c r="V19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="W19" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="W19" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>54</v>
@@ -4234,7 +4231,7 @@
         <v>90</v>
       </c>
       <c r="AH19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI19" s="2" t="s">
         <v>113</v>
@@ -4293,10 +4290,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>53</v>
@@ -4308,7 +4305,7 @@
         <v>54</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>56</v>
@@ -4377,7 +4374,7 @@
         <v>67</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE20" s="2" t="s">
         <v>68</v>
@@ -4448,13 +4445,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>54</v>
@@ -4532,7 +4529,7 @@
         <v>101</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE21" s="2" t="s">
         <v>68</v>
@@ -4541,10 +4538,10 @@
         <v>68</v>
       </c>
       <c r="AG21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH21" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="AH21" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="AI21" s="2" t="s">
         <v>91</v>
@@ -4553,7 +4550,7 @@
         <v>54</v>
       </c>
       <c r="AK21" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL21" s="2" t="s">
         <v>74</v>
@@ -4603,13 +4600,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>54</v>
@@ -4687,7 +4684,7 @@
         <v>89</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE22" s="2" t="s">
         <v>68</v>
@@ -4726,7 +4723,7 @@
         <v>120</v>
       </c>
       <c r="AQ22" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR22" s="2" t="s">
         <v>60</v>
@@ -4758,7 +4755,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>106</v>
@@ -4773,7 +4770,7 @@
         <v>54</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>56</v>
@@ -4791,7 +4788,7 @@
         <v>58</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>60</v>
@@ -4827,7 +4824,7 @@
         <v>87</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z23" s="2" t="s">
         <v>88</v>
@@ -4857,16 +4854,16 @@
         <v>72</v>
       </c>
       <c r="AI23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL23" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="AJ23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL23" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="AM23" s="2" t="s">
         <v>68</v>
@@ -4913,10 +4910,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>81</v>
@@ -4928,7 +4925,7 @@
         <v>54</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>56</v>
@@ -4997,7 +4994,7 @@
         <v>89</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE24" s="2" t="s">
         <v>68</v>
@@ -5006,13 +5003,13 @@
         <v>68</v>
       </c>
       <c r="AG24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH24" s="2" t="s">
         <v>102</v>
       </c>
       <c r="AI24" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ24" s="2" t="s">
         <v>60</v>
@@ -5068,10 +5065,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>81</v>
@@ -5083,7 +5080,7 @@
         <v>54</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>56</v>
@@ -5134,7 +5131,7 @@
         <v>63</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y25" s="2" t="s">
         <v>54</v>
@@ -5223,10 +5220,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>53</v>
@@ -5238,7 +5235,7 @@
         <v>54</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>56</v>
@@ -5322,7 +5319,7 @@
         <v>72</v>
       </c>
       <c r="AI26" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AJ26" s="2" t="s">
         <v>60</v>
@@ -5378,10 +5375,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>53</v>
@@ -5393,7 +5390,7 @@
         <v>54</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>83</v>
@@ -5411,7 +5408,7 @@
         <v>85</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>54</v>
@@ -5462,7 +5459,7 @@
         <v>67</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE27" s="2" t="s">
         <v>69</v>
@@ -5474,7 +5471,7 @@
         <v>90</v>
       </c>
       <c r="AH27" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI27" s="2" t="s">
         <v>73</v>
@@ -5501,7 +5498,7 @@
         <v>62</v>
       </c>
       <c r="AQ27" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR27" s="2" t="s">
         <v>60</v>
@@ -5533,10 +5530,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>53</v>
@@ -5548,7 +5545,7 @@
         <v>54</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>56</v>
@@ -5566,7 +5563,7 @@
         <v>58</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>178</v>
+        <v>54</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>54</v>
@@ -5617,7 +5614,7 @@
         <v>67</v>
       </c>
       <c r="AD28" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE28" s="2" t="s">
         <v>69</v>
@@ -5626,7 +5623,7 @@
         <v>70</v>
       </c>
       <c r="AG28" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AH28" s="2" t="s">
         <v>68</v>
@@ -5665,7 +5662,7 @@
         <v>54</v>
       </c>
       <c r="AT28" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU28" s="2" t="s">
         <v>68</v>
@@ -5688,13 +5685,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>54</v>
@@ -5703,7 +5700,7 @@
         <v>60</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>83</v>
@@ -5754,10 +5751,10 @@
         <v>63</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z29" s="2" t="s">
         <v>108</v>
@@ -5781,10 +5778,10 @@
         <v>68</v>
       </c>
       <c r="AG29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH29" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI29" s="2" t="s">
         <v>91</v>
@@ -5793,7 +5790,7 @@
         <v>54</v>
       </c>
       <c r="AK29" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL29" s="2" t="s">
         <v>68</v>
@@ -5843,13 +5840,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>54</v>
@@ -5909,10 +5906,10 @@
         <v>63</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z30" s="2" t="s">
         <v>108</v>
@@ -5936,10 +5933,10 @@
         <v>68</v>
       </c>
       <c r="AG30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI30" s="2" t="s">
         <v>91</v>
@@ -5948,10 +5945,10 @@
         <v>54</v>
       </c>
       <c r="AK30" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM30" s="2" t="s">
         <v>103</v>
@@ -5966,7 +5963,7 @@
         <v>104</v>
       </c>
       <c r="AQ30" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AR30" s="2" t="s">
         <v>68</v>
@@ -5975,7 +5972,7 @@
         <v>68</v>
       </c>
       <c r="AT30" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU30" s="2" t="s">
         <v>68</v>
@@ -5998,14 +5995,14 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="E31" s="2" t="s">
         <v>60</v>
       </c>
@@ -6013,7 +6010,7 @@
         <v>68</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>83</v>
@@ -6064,10 +6061,10 @@
         <v>63</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y31" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z31" s="2" t="s">
         <v>108</v>
@@ -6091,10 +6088,10 @@
         <v>68</v>
       </c>
       <c r="AG31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI31" s="2" t="s">
         <v>91</v>
@@ -6103,10 +6100,10 @@
         <v>54</v>
       </c>
       <c r="AK31" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL31" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM31" s="2" t="s">
         <v>68</v>
@@ -6153,13 +6150,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>60</v>
@@ -6219,10 +6216,10 @@
         <v>63</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z32" s="2" t="s">
         <v>108</v>
@@ -6246,7 +6243,7 @@
         <v>68</v>
       </c>
       <c r="AG32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH32" s="2" t="s">
         <v>68</v>
@@ -6294,7 +6291,7 @@
         <v>68</v>
       </c>
       <c r="AW32" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX32" s="2" t="s">
         <v>60</v>
@@ -6308,14 +6305,14 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="E33" s="2" t="s">
         <v>60</v>
       </c>
@@ -6323,7 +6320,7 @@
         <v>68</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>83</v>
@@ -6374,10 +6371,10 @@
         <v>63</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z33" s="2" t="s">
         <v>108</v>
@@ -6401,10 +6398,10 @@
         <v>68</v>
       </c>
       <c r="AG33" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH33" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI33" s="2" t="s">
         <v>91</v>
@@ -6413,10 +6410,10 @@
         <v>54</v>
       </c>
       <c r="AK33" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL33" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM33" s="2" t="s">
         <v>103</v>
@@ -6440,7 +6437,7 @@
         <v>68</v>
       </c>
       <c r="AT33" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU33" s="2" t="s">
         <v>68</v>
@@ -6463,7 +6460,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>106</v>
@@ -6478,7 +6475,7 @@
         <v>54</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>56</v>
@@ -6535,7 +6532,7 @@
         <v>117</v>
       </c>
       <c r="Z34" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA34" s="2" t="s">
         <v>54</v>
@@ -6547,19 +6544,19 @@
         <v>89</v>
       </c>
       <c r="AD34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH34" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="AE34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG34" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AH34" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="AI34" s="2" t="s">
         <v>91</v>
@@ -6583,7 +6580,7 @@
         <v>60</v>
       </c>
       <c r="AP34" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AQ34" s="2" t="s">
         <v>76</v>
@@ -6595,7 +6592,7 @@
         <v>68</v>
       </c>
       <c r="AT34" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU34" s="2" t="s">
         <v>68</v>
@@ -6618,10 +6615,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>81</v>
@@ -6773,10 +6770,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>81</v>
@@ -6928,7 +6925,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>98</v>
@@ -7012,7 +7009,7 @@
         <v>89</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE37" s="2" t="s">
         <v>68</v>
@@ -7024,7 +7021,7 @@
         <v>90</v>
       </c>
       <c r="AH37" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI37" s="2" t="s">
         <v>91</v>
@@ -7033,7 +7030,7 @@
         <v>54</v>
       </c>
       <c r="AK37" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL37" s="2" t="s">
         <v>74</v>
@@ -7051,7 +7048,7 @@
         <v>68</v>
       </c>
       <c r="AQ37" s="2" t="s">
-        <v>189</v>
+        <v>76</v>
       </c>
       <c r="AR37" s="2" t="s">
         <v>60</v>
@@ -7083,10 +7080,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>81</v>
@@ -7098,7 +7095,7 @@
         <v>54</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>56</v>
@@ -7176,10 +7173,10 @@
         <v>68</v>
       </c>
       <c r="AG38" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI38" s="2" t="s">
         <v>91</v>
@@ -7191,7 +7188,7 @@
         <v>54</v>
       </c>
       <c r="AL38" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM38" s="2" t="s">
         <v>54</v>
@@ -7238,13 +7235,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>54</v>
@@ -7253,7 +7250,7 @@
         <v>54</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>56</v>
@@ -7331,10 +7328,10 @@
         <v>68</v>
       </c>
       <c r="AG39" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH39" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI39" s="2" t="s">
         <v>113</v>
@@ -7358,7 +7355,7 @@
         <v>54</v>
       </c>
       <c r="AP39" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AQ39" s="2" t="s">
         <v>76</v>
@@ -7393,22 +7390,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>83</v>
@@ -7465,7 +7462,7 @@
         <v>117</v>
       </c>
       <c r="Z40" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA40" s="2" t="s">
         <v>60</v>
@@ -7477,7 +7474,7 @@
         <v>89</v>
       </c>
       <c r="AD40" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE40" s="2" t="s">
         <v>68</v>
@@ -7489,7 +7486,7 @@
         <v>90</v>
       </c>
       <c r="AH40" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI40" s="2" t="s">
         <v>91</v>
@@ -7516,7 +7513,7 @@
         <v>120</v>
       </c>
       <c r="AQ40" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR40" s="2" t="s">
         <v>60</v>
@@ -7525,7 +7522,7 @@
         <v>68</v>
       </c>
       <c r="AT40" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU40" s="2" t="s">
         <v>68</v>
@@ -7534,7 +7531,7 @@
         <v>68</v>
       </c>
       <c r="AW40" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX40" s="2" t="s">
         <v>60</v>
@@ -7548,7 +7545,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>98</v>
@@ -7611,7 +7608,7 @@
         <v>62</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>54</v>
@@ -7632,7 +7629,7 @@
         <v>101</v>
       </c>
       <c r="AD41" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE41" s="2" t="s">
         <v>111</v>
@@ -7644,7 +7641,7 @@
         <v>71</v>
       </c>
       <c r="AH41" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI41" s="2" t="s">
         <v>91</v>
@@ -7703,10 +7700,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>53</v>
@@ -7769,7 +7766,7 @@
         <v>63</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y42" s="2" t="s">
         <v>54</v>
@@ -7858,10 +7855,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>53</v>
@@ -7957,7 +7954,7 @@
         <v>72</v>
       </c>
       <c r="AI43" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ43" s="2" t="s">
         <v>60</v>
@@ -8013,13 +8010,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>54</v>
@@ -8028,7 +8025,7 @@
         <v>54</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>56</v>
@@ -8046,7 +8043,7 @@
         <v>58</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>54</v>
@@ -8085,7 +8082,7 @@
         <v>117</v>
       </c>
       <c r="Z44" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AA44" s="2" t="s">
         <v>60</v>
@@ -8097,7 +8094,7 @@
         <v>101</v>
       </c>
       <c r="AD44" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE44" s="2" t="s">
         <v>68</v>
@@ -8106,7 +8103,7 @@
         <v>68</v>
       </c>
       <c r="AG44" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH44" s="2" t="s">
         <v>102</v>
@@ -8121,7 +8118,7 @@
         <v>92</v>
       </c>
       <c r="AL44" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM44" s="2" t="s">
         <v>54</v>
@@ -8136,7 +8133,7 @@
         <v>68</v>
       </c>
       <c r="AQ44" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR44" s="2" t="s">
         <v>68</v>
@@ -8168,10 +8165,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>81</v>
@@ -8252,7 +8249,7 @@
         <v>101</v>
       </c>
       <c r="AD45" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE45" s="2" t="s">
         <v>68</v>
@@ -8264,7 +8261,7 @@
         <v>71</v>
       </c>
       <c r="AH45" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI45" s="2" t="s">
         <v>91</v>
@@ -8273,7 +8270,7 @@
         <v>54</v>
       </c>
       <c r="AK45" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL45" s="2" t="s">
         <v>74</v>
@@ -8323,13 +8320,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>54</v>
@@ -8356,7 +8353,7 @@
         <v>59</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>54</v>
@@ -8407,7 +8404,7 @@
         <v>101</v>
       </c>
       <c r="AD46" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE46" s="2" t="s">
         <v>68</v>
@@ -8416,10 +8413,10 @@
         <v>68</v>
       </c>
       <c r="AG46" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH46" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI46" s="2" t="s">
         <v>91</v>
@@ -8431,7 +8428,7 @@
         <v>95</v>
       </c>
       <c r="AL46" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM46" s="2" t="s">
         <v>68</v>
@@ -8455,7 +8452,7 @@
         <v>68</v>
       </c>
       <c r="AT46" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU46" s="2" t="s">
         <v>68</v>
@@ -8478,7 +8475,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>98</v>
@@ -8547,7 +8544,7 @@
         <v>87</v>
       </c>
       <c r="Y47" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z47" s="2" t="s">
         <v>88</v>
@@ -8562,7 +8559,7 @@
         <v>89</v>
       </c>
       <c r="AD47" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE47" s="2" t="s">
         <v>68</v>
@@ -8577,7 +8574,7 @@
         <v>102</v>
       </c>
       <c r="AI47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AJ47" s="2" t="s">
         <v>54</v>
@@ -8586,7 +8583,7 @@
         <v>95</v>
       </c>
       <c r="AL47" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM47" s="2" t="s">
         <v>68</v>
@@ -8633,7 +8630,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>52</v>
@@ -8648,7 +8645,7 @@
         <v>54</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>56</v>
@@ -8666,7 +8663,7 @@
         <v>59</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>54</v>
@@ -8702,7 +8699,7 @@
         <v>87</v>
       </c>
       <c r="Y48" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z48" s="2" t="s">
         <v>65</v>
@@ -8714,7 +8711,7 @@
         <v>66</v>
       </c>
       <c r="AC48" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD48" s="2" t="s">
         <v>68</v>
@@ -8732,13 +8729,13 @@
         <v>102</v>
       </c>
       <c r="AI48" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ48" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AK48" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL48" s="2" t="s">
         <v>74</v>
@@ -8788,10 +8785,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>53</v>
@@ -8803,7 +8800,7 @@
         <v>54</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>56</v>
@@ -8821,7 +8818,7 @@
         <v>58</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>60</v>
@@ -8854,7 +8851,7 @@
         <v>63</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y49" s="2" t="s">
         <v>54</v>
@@ -8887,7 +8884,7 @@
         <v>72</v>
       </c>
       <c r="AI49" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ49" s="2" t="s">
         <v>60</v>
@@ -8943,10 +8940,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>53</v>
@@ -8958,7 +8955,7 @@
         <v>54</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>56</v>
@@ -9051,7 +9048,7 @@
         <v>54</v>
       </c>
       <c r="AL50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM50" s="2" t="s">
         <v>54</v>
@@ -9075,7 +9072,7 @@
         <v>54</v>
       </c>
       <c r="AT50" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU50" s="2" t="s">
         <v>68</v>
@@ -9098,10 +9095,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>53</v>
@@ -9131,7 +9128,7 @@
         <v>58</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>60</v>
@@ -9164,7 +9161,7 @@
         <v>63</v>
       </c>
       <c r="X51" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y51" s="2" t="s">
         <v>54</v>
@@ -9197,7 +9194,7 @@
         <v>72</v>
       </c>
       <c r="AI51" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AJ51" s="2" t="s">
         <v>60</v>
@@ -9253,7 +9250,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>98</v>
@@ -9322,7 +9319,7 @@
         <v>54</v>
       </c>
       <c r="Y52" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z52" s="2" t="s">
         <v>62</v>
@@ -9408,13 +9405,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>54</v>
@@ -9492,7 +9489,7 @@
         <v>101</v>
       </c>
       <c r="AD53" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE53" s="2" t="s">
         <v>68</v>
@@ -9501,10 +9498,10 @@
         <v>68</v>
       </c>
       <c r="AG53" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH53" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI53" s="2" t="s">
         <v>113</v>
@@ -9516,7 +9513,7 @@
         <v>54</v>
       </c>
       <c r="AL53" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM53" s="2" t="s">
         <v>68</v>
@@ -9563,14 +9560,14 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="E54" s="2" t="s">
         <v>54</v>
       </c>
@@ -9578,7 +9575,7 @@
         <v>54</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>56</v>
@@ -9626,7 +9623,7 @@
         <v>62</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="X54" s="2" t="s">
         <v>87</v>
@@ -9662,7 +9659,7 @@
         <v>102</v>
       </c>
       <c r="AI54" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AJ54" s="2" t="s">
         <v>60</v>
@@ -9683,7 +9680,7 @@
         <v>54</v>
       </c>
       <c r="AP54" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AQ54" s="2" t="s">
         <v>76</v>
@@ -9695,7 +9692,7 @@
         <v>54</v>
       </c>
       <c r="AT54" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU54" s="2" t="s">
         <v>68</v>
@@ -9718,13 +9715,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>54</v>
@@ -9781,7 +9778,7 @@
         <v>60</v>
       </c>
       <c r="W55" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="X55" s="2" t="s">
         <v>54</v>
@@ -9811,10 +9808,10 @@
         <v>68</v>
       </c>
       <c r="AG55" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH55" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI55" s="2" t="s">
         <v>91</v>
@@ -9826,7 +9823,7 @@
         <v>68</v>
       </c>
       <c r="AL55" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM55" s="2" t="s">
         <v>54</v>
@@ -9873,13 +9870,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>60</v>
@@ -9888,7 +9885,7 @@
         <v>68</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>56</v>
@@ -9906,7 +9903,7 @@
         <v>59</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>54</v>
@@ -9957,7 +9954,7 @@
         <v>89</v>
       </c>
       <c r="AD56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE56" s="2" t="s">
         <v>68</v>
@@ -9966,7 +9963,7 @@
         <v>68</v>
       </c>
       <c r="AG56" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH56" s="2" t="s">
         <v>102</v>
@@ -9981,7 +9978,7 @@
         <v>62</v>
       </c>
       <c r="AL56" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM56" s="2" t="s">
         <v>54</v>
@@ -10005,7 +10002,7 @@
         <v>54</v>
       </c>
       <c r="AT56" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU56" s="2" t="s">
         <v>68</v>
@@ -10028,22 +10025,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>56</v>
@@ -10100,7 +10097,7 @@
         <v>117</v>
       </c>
       <c r="Z57" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA57" s="2" t="s">
         <v>60</v>
@@ -10124,7 +10121,7 @@
         <v>71</v>
       </c>
       <c r="AH57" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI57" s="2" t="s">
         <v>91</v>
@@ -10133,7 +10130,7 @@
         <v>54</v>
       </c>
       <c r="AK57" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL57" s="2" t="s">
         <v>74</v>
@@ -10169,7 +10166,7 @@
         <v>68</v>
       </c>
       <c r="AW57" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX57" s="2" t="s">
         <v>68</v>
@@ -10183,13 +10180,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>54</v>
@@ -10267,7 +10264,7 @@
         <v>101</v>
       </c>
       <c r="AD58" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE58" s="2" t="s">
         <v>68</v>
@@ -10315,7 +10312,7 @@
         <v>54</v>
       </c>
       <c r="AT58" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU58" s="2" t="s">
         <v>68</v>
@@ -10338,13 +10335,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>60</v>
@@ -10353,7 +10350,7 @@
         <v>68</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>56</v>
@@ -10422,7 +10419,7 @@
         <v>101</v>
       </c>
       <c r="AD59" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE59" s="2" t="s">
         <v>68</v>
@@ -10470,7 +10467,7 @@
         <v>68</v>
       </c>
       <c r="AT59" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU59" s="2" t="s">
         <v>68</v>
@@ -10493,13 +10490,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>54</v>
@@ -10589,7 +10586,7 @@
         <v>90</v>
       </c>
       <c r="AH60" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI60" s="2" t="s">
         <v>91</v>
@@ -10598,10 +10595,10 @@
         <v>54</v>
       </c>
       <c r="AK60" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL60" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM60" s="2" t="s">
         <v>54</v>
@@ -10625,7 +10622,7 @@
         <v>68</v>
       </c>
       <c r="AT60" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU60" s="2" t="s">
         <v>68</v>
@@ -10648,10 +10645,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>81</v>
@@ -10744,7 +10741,7 @@
         <v>71</v>
       </c>
       <c r="AH61" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI61" s="2" t="s">
         <v>91</v>
@@ -10803,7 +10800,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>78</v>
@@ -10887,7 +10884,7 @@
         <v>101</v>
       </c>
       <c r="AD62" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE62" s="2" t="s">
         <v>68</v>
@@ -10899,7 +10896,7 @@
         <v>71</v>
       </c>
       <c r="AH62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI62" s="2" t="s">
         <v>91</v>
@@ -10958,13 +10955,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>54</v>
@@ -10973,7 +10970,7 @@
         <v>54</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>56</v>
@@ -11042,7 +11039,7 @@
         <v>101</v>
       </c>
       <c r="AD63" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE63" s="2" t="s">
         <v>68</v>
@@ -11090,7 +11087,7 @@
         <v>68</v>
       </c>
       <c r="AT63" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU63" s="2" t="s">
         <v>68</v>
@@ -11113,10 +11110,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>53</v>
@@ -11128,7 +11125,7 @@
         <v>54</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>56</v>
@@ -11197,7 +11194,7 @@
         <v>101</v>
       </c>
       <c r="AD64" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE64" s="2" t="s">
         <v>68</v>
@@ -11209,7 +11206,7 @@
         <v>71</v>
       </c>
       <c r="AH64" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI64" s="2" t="s">
         <v>91</v>
@@ -11221,7 +11218,7 @@
         <v>95</v>
       </c>
       <c r="AL64" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM64" s="2" t="s">
         <v>54</v>
@@ -11245,7 +11242,7 @@
         <v>54</v>
       </c>
       <c r="AT64" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU64" s="2" t="s">
         <v>68</v>
@@ -11268,13 +11265,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>54</v>
@@ -11334,13 +11331,13 @@
         <v>63</v>
       </c>
       <c r="X65" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y65" s="2" t="s">
         <v>117</v>
       </c>
       <c r="Z65" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA65" s="2" t="s">
         <v>60</v>
@@ -11352,7 +11349,7 @@
         <v>89</v>
       </c>
       <c r="AD65" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE65" s="2" t="s">
         <v>68</v>
@@ -11361,10 +11358,10 @@
         <v>68</v>
       </c>
       <c r="AG65" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH65" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI65" s="2" t="s">
         <v>91</v>
@@ -11373,10 +11370,10 @@
         <v>54</v>
       </c>
       <c r="AK65" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL65" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM65" s="2" t="s">
         <v>103</v>
@@ -11391,7 +11388,7 @@
         <v>68</v>
       </c>
       <c r="AQ65" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR65" s="2" t="s">
         <v>68</v>
@@ -11400,7 +11397,7 @@
         <v>68</v>
       </c>
       <c r="AT65" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU65" s="2" t="s">
         <v>68</v>
@@ -11423,13 +11420,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>60</v>
@@ -11438,7 +11435,7 @@
         <v>68</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>83</v>
@@ -11489,13 +11486,13 @@
         <v>63</v>
       </c>
       <c r="X66" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y66" s="2" t="s">
         <v>117</v>
       </c>
       <c r="Z66" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA66" s="2" t="s">
         <v>60</v>
@@ -11507,7 +11504,7 @@
         <v>89</v>
       </c>
       <c r="AD66" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE66" s="2" t="s">
         <v>68</v>
@@ -11516,10 +11513,10 @@
         <v>68</v>
       </c>
       <c r="AG66" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH66" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI66" s="2" t="s">
         <v>91</v>
@@ -11528,10 +11525,10 @@
         <v>54</v>
       </c>
       <c r="AK66" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL66" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM66" s="2" t="s">
         <v>103</v>
@@ -11546,7 +11543,7 @@
         <v>68</v>
       </c>
       <c r="AQ66" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR66" s="2" t="s">
         <v>68</v>
@@ -11555,7 +11552,7 @@
         <v>68</v>
       </c>
       <c r="AT66" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU66" s="2" t="s">
         <v>68</v>
@@ -11578,13 +11575,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>54</v>
@@ -11671,10 +11668,10 @@
         <v>68</v>
       </c>
       <c r="AG67" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH67" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AI67" s="2" t="s">
         <v>91</v>
@@ -11686,7 +11683,7 @@
         <v>54</v>
       </c>
       <c r="AL67" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM67" s="2" t="s">
         <v>54</v>
@@ -11710,7 +11707,7 @@
         <v>68</v>
       </c>
       <c r="AT67" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU67" s="2" t="s">
         <v>68</v>
@@ -11719,7 +11716,7 @@
         <v>68</v>
       </c>
       <c r="AW67" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX67" s="2" t="s">
         <v>60</v>
@@ -11733,10 +11730,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>53</v>
@@ -11799,7 +11796,7 @@
         <v>63</v>
       </c>
       <c r="X68" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Y68" s="2" t="s">
         <v>117</v>
@@ -11814,7 +11811,7 @@
         <v>100</v>
       </c>
       <c r="AC68" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD68" s="2" t="s">
         <v>110</v>
@@ -11829,7 +11826,7 @@
         <v>90</v>
       </c>
       <c r="AH68" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI68" s="2" t="s">
         <v>91</v>
@@ -11838,7 +11835,7 @@
         <v>54</v>
       </c>
       <c r="AK68" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL68" s="2" t="s">
         <v>74</v>
@@ -11856,7 +11853,7 @@
         <v>104</v>
       </c>
       <c r="AQ68" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR68" s="2" t="s">
         <v>60</v>
@@ -11865,7 +11862,7 @@
         <v>54</v>
       </c>
       <c r="AT68" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU68" s="2" t="s">
         <v>68</v>
@@ -11874,7 +11871,7 @@
         <v>68</v>
       </c>
       <c r="AW68" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX68" s="2" t="s">
         <v>60</v>
@@ -11888,10 +11885,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>81</v>
@@ -11903,7 +11900,7 @@
         <v>54</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>56</v>
@@ -11948,7 +11945,7 @@
         <v>60</v>
       </c>
       <c r="V69" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="W69" s="2" t="s">
         <v>63</v>
@@ -11957,7 +11954,7 @@
         <v>87</v>
       </c>
       <c r="Y69" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z69" s="2" t="s">
         <v>108</v>
@@ -11987,7 +11984,7 @@
         <v>102</v>
       </c>
       <c r="AI69" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AJ69" s="2" t="s">
         <v>60</v>
@@ -12020,7 +12017,7 @@
         <v>54</v>
       </c>
       <c r="AT69" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU69" s="2" t="s">
         <v>68</v>
@@ -12029,7 +12026,7 @@
         <v>68</v>
       </c>
       <c r="AW69" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX69" s="2" t="s">
         <v>60</v>
@@ -12043,7 +12040,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>98</v>
@@ -12106,7 +12103,7 @@
         <v>62</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X70" s="2" t="s">
         <v>87</v>
@@ -12127,7 +12124,7 @@
         <v>101</v>
       </c>
       <c r="AD70" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE70" s="2" t="s">
         <v>111</v>
@@ -12198,10 +12195,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>53</v>
@@ -12321,7 +12318,7 @@
         <v>104</v>
       </c>
       <c r="AQ71" s="2" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="AR71" s="2" t="s">
         <v>60</v>
@@ -12330,7 +12327,7 @@
         <v>54</v>
       </c>
       <c r="AT71" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU71" s="2" t="s">
         <v>54</v>
@@ -12353,10 +12350,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>53</v>
@@ -12508,13 +12505,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>54</v>
@@ -12580,7 +12577,7 @@
         <v>54</v>
       </c>
       <c r="Z73" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AA73" s="2" t="s">
         <v>54</v>
@@ -12601,10 +12598,10 @@
         <v>68</v>
       </c>
       <c r="AG73" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AH73" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="AH73" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="AI73" s="2" t="s">
         <v>91</v>
@@ -12613,7 +12610,7 @@
         <v>54</v>
       </c>
       <c r="AK73" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL73" s="2" t="s">
         <v>74</v>
@@ -12640,7 +12637,7 @@
         <v>68</v>
       </c>
       <c r="AT73" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU73" s="2" t="s">
         <v>68</v>
@@ -12649,7 +12646,7 @@
         <v>68</v>
       </c>
       <c r="AW73" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX73" s="2" t="s">
         <v>54</v>
@@ -12663,7 +12660,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>98</v>
@@ -12732,7 +12729,7 @@
         <v>87</v>
       </c>
       <c r="Y74" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z74" s="2" t="s">
         <v>88</v>
@@ -12747,7 +12744,7 @@
         <v>89</v>
       </c>
       <c r="AD74" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE74" s="2" t="s">
         <v>68</v>
@@ -12768,10 +12765,10 @@
         <v>54</v>
       </c>
       <c r="AK74" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL74" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM74" s="2" t="s">
         <v>103</v>
@@ -12795,7 +12792,7 @@
         <v>68</v>
       </c>
       <c r="AT74" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU74" s="2" t="s">
         <v>68</v>
@@ -12804,7 +12801,7 @@
         <v>68</v>
       </c>
       <c r="AW74" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AX74" s="2" t="s">
         <v>54</v>
@@ -12818,13 +12815,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>54</v>
@@ -12902,7 +12899,7 @@
         <v>67</v>
       </c>
       <c r="AD75" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE75" s="2" t="s">
         <v>68</v>
@@ -12914,7 +12911,7 @@
         <v>90</v>
       </c>
       <c r="AH75" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI75" s="2" t="s">
         <v>91</v>
@@ -12950,7 +12947,7 @@
         <v>68</v>
       </c>
       <c r="AT75" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AU75" s="2" t="s">
         <v>68</v>
@@ -12973,13 +12970,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>54</v>
@@ -12988,7 +12985,7 @@
         <v>54</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>56</v>
@@ -13006,7 +13003,7 @@
         <v>59</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>54</v>
@@ -13057,7 +13054,7 @@
         <v>101</v>
       </c>
       <c r="AD76" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE76" s="2" t="s">
         <v>68</v>
@@ -13066,10 +13063,10 @@
         <v>68</v>
       </c>
       <c r="AG76" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AH76" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI76" s="2" t="s">
         <v>113</v>
@@ -13081,7 +13078,7 @@
         <v>95</v>
       </c>
       <c r="AL76" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM76" s="2" t="s">
         <v>68</v>
@@ -13105,7 +13102,7 @@
         <v>68</v>
       </c>
       <c r="AT76" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU76" s="2" t="s">
         <v>68</v>
@@ -13128,13 +13125,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>54</v>
@@ -13212,7 +13209,7 @@
         <v>101</v>
       </c>
       <c r="AD77" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE77" s="2" t="s">
         <v>68</v>
@@ -13233,10 +13230,10 @@
         <v>54</v>
       </c>
       <c r="AK77" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL77" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM77" s="2" t="s">
         <v>54</v>
@@ -13260,7 +13257,7 @@
         <v>54</v>
       </c>
       <c r="AT77" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AU77" s="2" t="s">
         <v>68</v>
@@ -13283,10 +13280,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>81</v>
@@ -13298,7 +13295,7 @@
         <v>54</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>83</v>
@@ -13352,7 +13349,7 @@
         <v>87</v>
       </c>
       <c r="Y78" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z78" s="2" t="s">
         <v>88</v>
@@ -13367,7 +13364,7 @@
         <v>89</v>
       </c>
       <c r="AD78" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE78" s="2" t="s">
         <v>68</v>
@@ -13379,7 +13376,7 @@
         <v>90</v>
       </c>
       <c r="AH78" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI78" s="2" t="s">
         <v>91</v>
@@ -13388,10 +13385,10 @@
         <v>54</v>
       </c>
       <c r="AK78" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL78" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM78" s="2" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Turning variables ordinal, leaving -values
I rechecked some values in the case db to make sure I didn't miscode them before turning the variable into an ordinal one. also first experiments with test data
</commit_message>
<xml_diff>
--- a/case codings database.xlsx
+++ b/case codings database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Studium\Bachelor's Thesis\ucf-thesis-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5862D81-14E2-4A92-A6D8-33CDD9F8C528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8866D9-BC03-4FB1-BCB1-DE2EF57EB75D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="-14955" windowWidth="23010" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="245">
   <si>
     <t>ID</t>
   </si>
@@ -555,9 +555,6 @@
     <t>Finogenov and Others v. Russia</t>
   </si>
   <si>
-    <t>1 = Lower</t>
-  </si>
-  <si>
     <t>2 = Higher</t>
   </si>
   <si>
@@ -757,6 +754,12 @@
   </si>
   <si>
     <t>1 = Yes, they considered or used alternative strategies before the use of force in question</t>
+  </si>
+  <si>
+    <t>1 = Unchanged</t>
+  </si>
+  <si>
+    <t>0 = Lower</t>
   </si>
 </sst>
 </file>
@@ -1326,8 +1329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM64" workbookViewId="0">
-      <selection activeCell="AQ44" sqref="AQ44"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,7 +1537,7 @@
         <v>58</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>60</v>
@@ -1688,7 +1692,7 @@
         <v>58</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>60</v>
@@ -1843,7 +1847,7 @@
         <v>58</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>60</v>
@@ -1998,7 +2002,7 @@
         <v>58</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>60</v>
@@ -2153,7 +2157,7 @@
         <v>85</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>60</v>
@@ -2308,7 +2312,7 @@
         <v>58</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>54</v>
@@ -2463,7 +2467,7 @@
         <v>58</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>54</v>
@@ -2553,7 +2557,7 @@
         <v>120</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR8" s="2" t="s">
         <v>60</v>
@@ -2618,7 +2622,7 @@
         <v>58</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>60</v>
@@ -2654,10 +2658,10 @@
         <v>62</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="AA9" s="2" t="s">
         <v>54</v>
@@ -2773,7 +2777,7 @@
         <v>58</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>54</v>
@@ -2928,7 +2932,7 @@
         <v>58</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>60</v>
@@ -3009,7 +3013,7 @@
         <v>68</v>
       </c>
       <c r="AN11" s="2" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="AO11" s="2" t="s">
         <v>68</v>
@@ -3083,7 +3087,7 @@
         <v>59</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>54</v>
@@ -3238,7 +3242,7 @@
         <v>59</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>54</v>
@@ -3393,7 +3397,7 @@
         <v>58</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>54</v>
@@ -3483,7 +3487,7 @@
         <v>120</v>
       </c>
       <c r="AQ14" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR14" s="2" t="s">
         <v>60</v>
@@ -3548,7 +3552,7 @@
         <v>58</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>60</v>
@@ -3593,10 +3597,10 @@
         <v>62</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="AD15" s="2" t="s">
         <v>68</v>
@@ -3703,7 +3707,7 @@
         <v>58</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>54</v>
@@ -3793,7 +3797,7 @@
         <v>120</v>
       </c>
       <c r="AQ16" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR16" s="2" t="s">
         <v>68</v>
@@ -3858,7 +3862,7 @@
         <v>85</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>54</v>
@@ -3948,7 +3952,7 @@
         <v>120</v>
       </c>
       <c r="AQ17" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR17" s="2" t="s">
         <v>60</v>
@@ -4013,7 +4017,7 @@
         <v>58</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>54</v>
@@ -4168,7 +4172,7 @@
         <v>58</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>54</v>
@@ -4207,7 +4211,7 @@
         <v>54</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="AA19" s="2" t="s">
         <v>54</v>
@@ -4323,7 +4327,7 @@
         <v>58</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>54</v>
@@ -4478,7 +4482,7 @@
         <v>58</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>54</v>
@@ -4633,7 +4637,7 @@
         <v>62</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>54</v>
@@ -4723,7 +4727,7 @@
         <v>120</v>
       </c>
       <c r="AQ22" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR22" s="2" t="s">
         <v>60</v>
@@ -4788,7 +4792,7 @@
         <v>58</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>60</v>
@@ -4943,7 +4947,7 @@
         <v>59</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>54</v>
@@ -4979,10 +4983,10 @@
         <v>62</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>62</v>
+        <v>167</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="AA24" s="2" t="s">
         <v>62</v>
@@ -5098,7 +5102,7 @@
         <v>58</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>60</v>
@@ -5137,7 +5141,7 @@
         <v>54</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="AA25" s="2" t="s">
         <v>54</v>
@@ -5253,7 +5257,7 @@
         <v>85</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>60</v>
@@ -5292,7 +5296,7 @@
         <v>54</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>62</v>
+        <v>235</v>
       </c>
       <c r="AA26" s="2" t="s">
         <v>62</v>
@@ -5408,7 +5412,7 @@
         <v>85</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>54</v>
@@ -5498,7 +5502,7 @@
         <v>62</v>
       </c>
       <c r="AQ27" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR27" s="2" t="s">
         <v>60</v>
@@ -5563,7 +5567,7 @@
         <v>58</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>54</v>
@@ -5662,7 +5666,7 @@
         <v>54</v>
       </c>
       <c r="AT28" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU28" s="2" t="s">
         <v>68</v>
@@ -5685,13 +5689,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>54</v>
@@ -5718,7 +5722,7 @@
         <v>58</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>54</v>
@@ -5840,13 +5844,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>54</v>
@@ -5873,7 +5877,7 @@
         <v>58</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>54</v>
@@ -5995,13 +5999,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>174</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>60</v>
@@ -6028,7 +6032,7 @@
         <v>58</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>54</v>
@@ -6150,13 +6154,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>174</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>60</v>
@@ -6183,7 +6187,7 @@
         <v>85</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>54</v>
@@ -6305,13 +6309,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>174</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>60</v>
@@ -6338,7 +6342,7 @@
         <v>58</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>54</v>
@@ -6460,7 +6464,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>106</v>
@@ -6493,7 +6497,7 @@
         <v>58</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>54</v>
@@ -6532,7 +6536,7 @@
         <v>117</v>
       </c>
       <c r="Z34" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA34" s="2" t="s">
         <v>54</v>
@@ -6580,7 +6584,7 @@
         <v>60</v>
       </c>
       <c r="AP34" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AQ34" s="2" t="s">
         <v>76</v>
@@ -6615,10 +6619,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>81</v>
@@ -6648,7 +6652,7 @@
         <v>58</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>54</v>
@@ -6687,7 +6691,7 @@
         <v>117</v>
       </c>
       <c r="Z35" s="2" t="s">
-        <v>62</v>
+        <v>235</v>
       </c>
       <c r="AA35" s="2" t="s">
         <v>54</v>
@@ -6770,7 +6774,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>171</v>
@@ -6803,7 +6807,7 @@
         <v>58</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>54</v>
@@ -6925,7 +6929,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>98</v>
@@ -6958,7 +6962,7 @@
         <v>85</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>54</v>
@@ -7080,7 +7084,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>122</v>
@@ -7113,7 +7117,7 @@
         <v>58</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>54</v>
@@ -7122,7 +7126,7 @@
         <v>54</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>60</v>
@@ -7152,7 +7156,7 @@
         <v>117</v>
       </c>
       <c r="Z38" s="2" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="AA38" s="2" t="s">
         <v>62</v>
@@ -7161,7 +7165,7 @@
         <v>100</v>
       </c>
       <c r="AC38" s="2" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="AD38" s="2" t="s">
         <v>68</v>
@@ -7235,13 +7239,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>54</v>
@@ -7268,7 +7272,7 @@
         <v>58</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>54</v>
@@ -7355,7 +7359,7 @@
         <v>54</v>
       </c>
       <c r="AP39" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AQ39" s="2" t="s">
         <v>76</v>
@@ -7390,22 +7394,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>83</v>
@@ -7423,7 +7427,7 @@
         <v>85</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>54</v>
@@ -7462,7 +7466,7 @@
         <v>117</v>
       </c>
       <c r="Z40" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA40" s="2" t="s">
         <v>60</v>
@@ -7513,7 +7517,7 @@
         <v>120</v>
       </c>
       <c r="AQ40" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR40" s="2" t="s">
         <v>60</v>
@@ -7545,7 +7549,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>98</v>
@@ -7578,7 +7582,7 @@
         <v>58</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N41" s="2" t="s">
         <v>54</v>
@@ -7700,7 +7704,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>150</v>
@@ -7733,7 +7737,7 @@
         <v>58</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>60</v>
@@ -7855,7 +7859,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>150</v>
@@ -7888,7 +7892,7 @@
         <v>58</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N43" s="2" t="s">
         <v>60</v>
@@ -8010,13 +8014,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>54</v>
@@ -8043,7 +8047,7 @@
         <v>58</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>54</v>
@@ -8082,7 +8086,7 @@
         <v>117</v>
       </c>
       <c r="Z44" s="2" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="AA44" s="2" t="s">
         <v>60</v>
@@ -8133,7 +8137,7 @@
         <v>68</v>
       </c>
       <c r="AQ44" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR44" s="2" t="s">
         <v>68</v>
@@ -8165,7 +8169,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>150</v>
@@ -8198,7 +8202,7 @@
         <v>58</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>54</v>
@@ -8320,7 +8324,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>78</v>
@@ -8353,7 +8357,7 @@
         <v>59</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>54</v>
@@ -8475,7 +8479,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>98</v>
@@ -8508,7 +8512,7 @@
         <v>85</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>54</v>
@@ -8630,7 +8634,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>52</v>
@@ -8663,7 +8667,7 @@
         <v>59</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>54</v>
@@ -8785,7 +8789,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>174</v>
@@ -8818,7 +8822,7 @@
         <v>58</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>60</v>
@@ -8940,7 +8944,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>165</v>
@@ -8973,7 +8977,7 @@
         <v>59</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>54</v>
@@ -9095,7 +9099,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>174</v>
@@ -9128,7 +9132,7 @@
         <v>58</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>60</v>
@@ -9250,7 +9254,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>98</v>
@@ -9283,7 +9287,7 @@
         <v>58</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>54</v>
@@ -9322,7 +9326,7 @@
         <v>167</v>
       </c>
       <c r="Z52" s="2" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="AA52" s="2" t="s">
         <v>54</v>
@@ -9405,13 +9409,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>54</v>
@@ -9438,7 +9442,7 @@
         <v>58</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>54</v>
@@ -9560,13 +9564,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>54</v>
@@ -9593,7 +9597,7 @@
         <v>58</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>54</v>
@@ -9623,7 +9627,7 @@
         <v>62</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="X54" s="2" t="s">
         <v>87</v>
@@ -9680,7 +9684,7 @@
         <v>54</v>
       </c>
       <c r="AP54" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AQ54" s="2" t="s">
         <v>76</v>
@@ -9692,7 +9696,7 @@
         <v>54</v>
       </c>
       <c r="AT54" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU54" s="2" t="s">
         <v>68</v>
@@ -9715,13 +9719,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>54</v>
@@ -9748,7 +9752,7 @@
         <v>59</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>54</v>
@@ -9870,13 +9874,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>60</v>
@@ -9903,7 +9907,7 @@
         <v>59</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>54</v>
@@ -10025,10 +10029,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>151</v>
@@ -10058,7 +10062,7 @@
         <v>85</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>54</v>
@@ -10097,7 +10101,7 @@
         <v>117</v>
       </c>
       <c r="Z57" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA57" s="2" t="s">
         <v>60</v>
@@ -10180,7 +10184,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>80</v>
@@ -10213,7 +10217,7 @@
         <v>58</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N58" s="2" t="s">
         <v>54</v>
@@ -10335,7 +10339,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>150</v>
@@ -10368,7 +10372,7 @@
         <v>59</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>54</v>
@@ -10490,7 +10494,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>122</v>
@@ -10523,7 +10527,7 @@
         <v>58</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>54</v>
@@ -10645,10 +10649,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>81</v>
@@ -10678,7 +10682,7 @@
         <v>58</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>54</v>
@@ -10800,7 +10804,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>78</v>
@@ -10833,7 +10837,7 @@
         <v>58</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N62" s="2" t="s">
         <v>54</v>
@@ -10955,13 +10959,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>54</v>
@@ -10988,7 +10992,7 @@
         <v>58</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>54</v>
@@ -11110,7 +11114,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>165</v>
@@ -11143,7 +11147,7 @@
         <v>59</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>54</v>
@@ -11265,13 +11269,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>54</v>
@@ -11298,7 +11302,7 @@
         <v>58</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N65" s="2" t="s">
         <v>54</v>
@@ -11337,7 +11341,7 @@
         <v>117</v>
       </c>
       <c r="Z65" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA65" s="2" t="s">
         <v>60</v>
@@ -11388,7 +11392,7 @@
         <v>68</v>
       </c>
       <c r="AQ65" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR65" s="2" t="s">
         <v>68</v>
@@ -11420,13 +11424,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>60</v>
@@ -11453,7 +11457,7 @@
         <v>58</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N66" s="2" t="s">
         <v>54</v>
@@ -11492,7 +11496,7 @@
         <v>117</v>
       </c>
       <c r="Z66" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA66" s="2" t="s">
         <v>60</v>
@@ -11543,7 +11547,7 @@
         <v>68</v>
       </c>
       <c r="AQ66" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR66" s="2" t="s">
         <v>68</v>
@@ -11575,10 +11579,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>146</v>
@@ -11608,7 +11612,7 @@
         <v>85</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>54</v>
@@ -11707,7 +11711,7 @@
         <v>68</v>
       </c>
       <c r="AT67" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU67" s="2" t="s">
         <v>68</v>
@@ -11730,7 +11734,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>131</v>
@@ -11763,7 +11767,7 @@
         <v>58</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N68" s="2" t="s">
         <v>54</v>
@@ -11796,7 +11800,7 @@
         <v>63</v>
       </c>
       <c r="X68" s="2" t="s">
-        <v>159</v>
+        <v>64</v>
       </c>
       <c r="Y68" s="2" t="s">
         <v>117</v>
@@ -11853,7 +11857,7 @@
         <v>104</v>
       </c>
       <c r="AQ68" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR68" s="2" t="s">
         <v>60</v>
@@ -11862,7 +11866,7 @@
         <v>54</v>
       </c>
       <c r="AT68" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU68" s="2" t="s">
         <v>68</v>
@@ -11885,7 +11889,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>150</v>
@@ -11918,7 +11922,7 @@
         <v>59</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N69" s="2" t="s">
         <v>54</v>
@@ -12040,7 +12044,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>98</v>
@@ -12073,7 +12077,7 @@
         <v>58</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>54</v>
@@ -12195,7 +12199,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>138</v>
@@ -12228,7 +12232,7 @@
         <v>58</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N71" s="2" t="s">
         <v>60</v>
@@ -12267,7 +12271,7 @@
         <v>54</v>
       </c>
       <c r="Z71" s="2" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="AA71" s="2" t="s">
         <v>60</v>
@@ -12318,7 +12322,7 @@
         <v>104</v>
       </c>
       <c r="AQ71" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR71" s="2" t="s">
         <v>60</v>
@@ -12327,7 +12331,7 @@
         <v>54</v>
       </c>
       <c r="AT71" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU71" s="2" t="s">
         <v>54</v>
@@ -12350,7 +12354,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>138</v>
@@ -12383,7 +12387,7 @@
         <v>59</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>60</v>
@@ -12422,7 +12426,7 @@
         <v>54</v>
       </c>
       <c r="Z72" s="2" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="AA72" s="2" t="s">
         <v>60</v>
@@ -12505,13 +12509,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>54</v>
@@ -12538,7 +12542,7 @@
         <v>59</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N73" s="2" t="s">
         <v>54</v>
@@ -12577,7 +12581,7 @@
         <v>54</v>
       </c>
       <c r="Z73" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA73" s="2" t="s">
         <v>54</v>
@@ -12660,7 +12664,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>98</v>
@@ -12693,7 +12697,7 @@
         <v>85</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N74" s="2" t="s">
         <v>54</v>
@@ -12815,7 +12819,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>78</v>
@@ -12848,7 +12852,7 @@
         <v>58</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>54</v>
@@ -12970,7 +12974,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>78</v>
@@ -13003,7 +13007,7 @@
         <v>59</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>54</v>
@@ -13102,7 +13106,7 @@
         <v>68</v>
       </c>
       <c r="AT76" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU76" s="2" t="s">
         <v>68</v>
@@ -13125,13 +13129,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>54</v>
@@ -13158,7 +13162,7 @@
         <v>58</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N77" s="2" t="s">
         <v>54</v>
@@ -13257,7 +13261,7 @@
         <v>54</v>
       </c>
       <c r="AT77" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AU77" s="2" t="s">
         <v>68</v>
@@ -13280,7 +13284,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>122</v>
@@ -13313,7 +13317,7 @@
         <v>85</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="N78" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Creating the figure versions of the prettified graphs
</commit_message>
<xml_diff>
--- a/case codings database.xlsx
+++ b/case codings database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Studium\Bachelor's Thesis\ucf-thesis-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8866D9-BC03-4FB1-BCB1-DE2EF57EB75D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E71D7B-A6E1-4E27-B047-9C6149DAA766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -972,7 +972,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AY78" totalsRowShown="0">
-  <autoFilter ref="A1:AY78" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A1:AY78" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="26">
+      <filters>
+        <filter val="1 = Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="51">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="50"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="case" dataDxfId="49"/>
@@ -1329,9 +1335,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1499,7 +1505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2274,7 +2280,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3204,7 +3210,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3979,7 +3985,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4289,7 +4295,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4909,7 +4915,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5064,7 +5070,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5219,7 +5225,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6459,7 +6465,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6614,7 +6620,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6769,7 +6775,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -7079,7 +7085,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7544,7 +7550,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7699,7 +7705,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -7854,7 +7860,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -8164,7 +8170,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -8629,7 +8635,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -8784,7 +8790,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8939,7 +8945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -9094,7 +9100,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -9249,7 +9255,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -9404,7 +9410,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -9559,7 +9565,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -10179,7 +10185,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -10334,7 +10340,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -10489,7 +10495,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -10644,7 +10650,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -10799,7 +10805,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -10954,7 +10960,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -11729,7 +11735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -11884,7 +11890,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -12039,7 +12045,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -12504,7 +12510,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -12814,7 +12820,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -12969,7 +12975,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:51" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>

</xml_diff>